<commit_message>
Update datos expresion de genes y sobrevivencia
</commit_message>
<xml_diff>
--- a/Datos/Datos expresion genica.xlsx
+++ b/Datos/Datos expresion genica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11012"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/fabianallende/Documents/GitHub/Bachelor_Thesis_Fabian_Allende/Memoria de Titulo II/Datos y calculos/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Dropbox/CURSOS/POSTGRADO/DBT_845_INVESTIGACION_REPRODUCIBLE/2022/Tarea_Daniela/Tarea_DL_DBT845/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D18372F8-9E97-C847-9A9A-DE3AB09D4AB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{492947E2-8FBF-D04B-B363-D024EE8A7879}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{680CF234-4357-984E-A769-9CE75CCE8B06}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16400" activeTab="3" xr2:uid="{680CF234-4357-984E-A769-9CE75CCE8B06}"/>
   </bookViews>
   <sheets>
     <sheet name="Phenotype" sheetId="1" r:id="rId1"/>
@@ -18,20 +18,14 @@
     <sheet name="CT value" sheetId="2" r:id="rId3"/>
     <sheet name="CT_PROM" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Phenotype!$A$1:$O$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'RNA extraction'!$A$1:$G$42</definedName>
+  </definedNames>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -1137,8 +1131,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CAB6050A-7FCA-9248-867E-14EDC945A103}">
   <dimension ref="A1:O43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:K1048576"/>
+    <sheetView zoomScale="110" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3003,7 +2997,8 @@
       <c r="A43" s="10"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O43">
+  <autoFilter ref="A1:O42" xr:uid="{47BA16CF-4A9E-DE42-BEE8-E9518D60F92D}"/>
+  <sortState ref="A2:O43">
     <sortCondition ref="A1:A43"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3017,8 +3012,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EF447F7-D1CC-0A4D-8D51-FAE51C0B0E5A}">
   <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView topLeftCell="A37" zoomScale="107" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+    <sheetView zoomScale="107" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3828,7 +3823,12 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:H42">
+  <autoFilter ref="A1:G42" xr:uid="{19F7FA05-2B36-094E-A17A-0C064121B695}">
+    <sortState ref="A2:G42">
+      <sortCondition ref="A1:A42"/>
+    </sortState>
+  </autoFilter>
+  <sortState ref="A2:H42">
     <sortCondition ref="A14:A42"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3840,7 +3840,7 @@
   <dimension ref="A1:CI42"/>
   <sheetViews>
     <sheetView zoomScale="137" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="Y12" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -14639,13 +14639,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E56242B-91FC-9244-A5EF-23688C07179B}">
   <dimension ref="A1:V42"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="104" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" zoomScale="104" workbookViewId="0">
+      <selection sqref="A1:A1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
+    <col min="2" max="2" width="19.33203125" customWidth="1"/>
     <col min="5" max="5" width="11.83203125" customWidth="1"/>
     <col min="6" max="6" width="11.5" customWidth="1"/>
     <col min="8" max="8" width="12.6640625" customWidth="1"/>

</xml_diff>